<commit_message>
Adding new version of "Tasks.xslx"
</commit_message>
<xml_diff>
--- a/src/Tasks.xlsx
+++ b/src/Tasks.xlsx
@@ -169,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -375,11 +375,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -448,12 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -467,6 +511,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -615,11 +686,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="128350080"/>
-        <c:axId val="128348544"/>
+        <c:axId val="76454144"/>
+        <c:axId val="76468992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="128350080"/>
+        <c:axId val="76454144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,12 +715,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128348544"/>
+        <c:crossAx val="76468992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="128348544"/>
+        <c:axId val="76468992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +746,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128350080"/>
+        <c:crossAx val="76454144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -684,7 +755,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1012,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J2147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1107,132 +1178,132 @@
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="31" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D5" s="19"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1">
       <c r="A6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="H6" s="15"/>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="19"/>
+        <v>14</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>32</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D8" s="19"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="H8" s="15"/>
       <c r="I8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
+      <c r="A9" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>14</v>
@@ -1252,20 +1323,20 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="4" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="35" t="s">
         <v>33</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1276,20 +1347,20 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A11" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="26" t="s">
+      <c r="A11" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="1" t="s">

</xml_diff>